<commit_message>
SCRIPT PARA NACIMIENTOS 2015-2016
NO SE NECESITARON CAMBIOS EN LAS BASES DE DATOS
</commit_message>
<xml_diff>
--- a/xlsx/AnalisisVariablesProyecto.xlsx
+++ b/xlsx/AnalisisVariablesProyecto.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\mineria de datos\ProyectoMineria1\Proyecto-analisis-y-clustering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\GIT\Proyecto-analisis-y-clustering\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D06A38E-4C5A-4D70-A0EC-85A4AEE2057A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AD27DE-3DE4-4D84-9F8D-0CD333D6058C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27195" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="106">
   <si>
     <t>Depreg</t>
   </si>
@@ -187,6 +188,162 @@
   </si>
   <si>
     <t>NUNUMU</t>
+  </si>
+  <si>
+    <t>DEPREG</t>
+  </si>
+  <si>
+    <t>MUPREG</t>
+  </si>
+  <si>
+    <t>MESREG</t>
+  </si>
+  <si>
+    <t>AÑOREG</t>
+  </si>
+  <si>
+    <t>CLAUNI</t>
+  </si>
+  <si>
+    <t>AÑOOCU</t>
+  </si>
+  <si>
+    <t>EDADHOM</t>
+  </si>
+  <si>
+    <t>EDADMUJ</t>
+  </si>
+  <si>
+    <t>NACHOM</t>
+  </si>
+  <si>
+    <t>NACMUJ</t>
+  </si>
+  <si>
+    <t>ESCHOM</t>
+  </si>
+  <si>
+    <t>ESCMUJ</t>
+  </si>
+  <si>
+    <t>DEPOCU</t>
+  </si>
+  <si>
+    <t>MUPOCU</t>
+  </si>
+  <si>
+    <t>DIAOCU</t>
+  </si>
+  <si>
+    <t>MESOCU</t>
+  </si>
+  <si>
+    <t>AREAGOCU</t>
+  </si>
+  <si>
+    <t>TIPOINS</t>
+  </si>
+  <si>
+    <t>LIBRAS</t>
+  </si>
+  <si>
+    <t>ONZAS</t>
+  </si>
+  <si>
+    <t>DIACOU</t>
+  </si>
+  <si>
+    <t>SEXO</t>
+  </si>
+  <si>
+    <t>TIPAR</t>
+  </si>
+  <si>
+    <t>VIAPAR</t>
+  </si>
+  <si>
+    <t>EDADP</t>
+  </si>
+  <si>
+    <t>PAISREP</t>
+  </si>
+  <si>
+    <t>DEPREP</t>
+  </si>
+  <si>
+    <t>MUPREP</t>
+  </si>
+  <si>
+    <t>PUEBLOPP</t>
+  </si>
+  <si>
+    <t>ESCIVP</t>
+  </si>
+  <si>
+    <t>PAISNACP</t>
+  </si>
+  <si>
+    <t>DEPNAP</t>
+  </si>
+  <si>
+    <t>MUNPNAP</t>
+  </si>
+  <si>
+    <t>ESCOLAP</t>
+  </si>
+  <si>
+    <t>OCUPAP</t>
+  </si>
+  <si>
+    <t>EDADM</t>
+  </si>
+  <si>
+    <t>PAISREM</t>
+  </si>
+  <si>
+    <t>DEPREM</t>
+  </si>
+  <si>
+    <t>MUPREM</t>
+  </si>
+  <si>
+    <t>PUEBLOPM</t>
+  </si>
+  <si>
+    <t>ESCIVM</t>
+  </si>
+  <si>
+    <t>PAISNACM</t>
+  </si>
+  <si>
+    <t>DEPNAM</t>
+  </si>
+  <si>
+    <t>MUPNAM</t>
+  </si>
+  <si>
+    <t>ESCOLAM</t>
+  </si>
+  <si>
+    <t>OCUPAM</t>
+  </si>
+  <si>
+    <t>ASISREC</t>
+  </si>
+  <si>
+    <t>SITIOOCU</t>
+  </si>
+  <si>
+    <t>TOHITE</t>
+  </si>
+  <si>
+    <t>TOHINM</t>
+  </si>
+  <si>
+    <t>TOHIVI</t>
+  </si>
+  <si>
+    <t>PURBLOPP</t>
   </si>
 </sst>
 </file>
@@ -303,8 +460,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -312,32 +475,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,794 +776,934 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:O32"/>
+  <dimension ref="A4:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="N6" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" customWidth="1"/>
-    <col min="15" max="15" width="28.5703125" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" customWidth="1"/>
+    <col min="15" max="15" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="16"/>
       <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="16"/>
       <c r="I4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="9"/>
+      <c r="K4" s="16"/>
       <c r="M4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="9"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O4" s="16"/>
+      <c r="Q4" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="11"/>
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="11"/>
       <c r="I5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="5"/>
+      <c r="K5" s="11"/>
       <c r="M5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O5" s="11"/>
+      <c r="Q5" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="11"/>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="11"/>
       <c r="I6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="5"/>
+      <c r="K6" s="11"/>
       <c r="M6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O6" s="11"/>
+      <c r="Q6" t="s">
+        <v>56</v>
+      </c>
+      <c r="S6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="11"/>
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="11"/>
       <c r="I7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="K7" s="11"/>
       <c r="M7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O7" s="11"/>
+      <c r="Q7" t="s">
+        <v>57</v>
+      </c>
+      <c r="S7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="11"/>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="11"/>
       <c r="I8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="K8" s="11"/>
       <c r="M8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O8" s="11"/>
+      <c r="Q8" t="s">
+        <v>58</v>
+      </c>
+      <c r="S8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="11"/>
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="11"/>
       <c r="I9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="K9" s="11"/>
       <c r="M9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O9" s="11"/>
+      <c r="Q9" t="s">
+        <v>60</v>
+      </c>
+      <c r="S9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="11"/>
       <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="11"/>
       <c r="I10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="5"/>
+      <c r="K10" s="11"/>
       <c r="M10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O10" s="11"/>
+      <c r="Q10" t="s">
+        <v>61</v>
+      </c>
+      <c r="S10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="11"/>
       <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="11"/>
       <c r="I11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="M11" s="13" t="s">
+      <c r="K11" s="9"/>
+      <c r="M11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="14"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O11" s="15"/>
+      <c r="Q11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="11"/>
       <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="11"/>
       <c r="I12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="M12" s="13" t="s">
+      <c r="K12" s="9"/>
+      <c r="M12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N12" s="14" t="s">
+      <c r="N12" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="O12" s="14"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O12" s="15"/>
+      <c r="Q12" t="s">
+        <v>45</v>
+      </c>
+      <c r="S12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="11"/>
       <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="11"/>
       <c r="I13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="6"/>
+      <c r="K13" s="8"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="11"/>
       <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="11"/>
       <c r="I14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="8"/>
       <c r="M14" s="3"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="11"/>
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="11"/>
       <c r="I15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="5"/>
+      <c r="K15" s="11"/>
       <c r="M15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O15" s="11"/>
+      <c r="Q15" t="s">
+        <v>62</v>
+      </c>
+      <c r="S15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="11"/>
       <c r="E16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="11"/>
       <c r="I16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="5"/>
+      <c r="K16" s="11"/>
       <c r="M16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O16" s="11"/>
+      <c r="Q16" t="s">
+        <v>63</v>
+      </c>
+      <c r="S16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="11"/>
       <c r="E17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="11"/>
       <c r="I17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="5"/>
+      <c r="K17" s="11"/>
       <c r="M17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O17" s="11"/>
+      <c r="Q17" t="s">
+        <v>64</v>
+      </c>
+      <c r="S17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="11"/>
       <c r="E18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="11"/>
       <c r="I18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="5"/>
+      <c r="K18" s="11"/>
       <c r="M18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O18" s="11"/>
+      <c r="Q18" t="s">
+        <v>65</v>
+      </c>
+      <c r="S18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="11"/>
       <c r="E19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="11"/>
       <c r="I19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="8"/>
+      <c r="K19" s="14"/>
       <c r="M19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N19" s="8" t="s">
+      <c r="N19" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="O19" s="8"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O19" s="14"/>
+      <c r="Q19" t="s">
+        <v>47</v>
+      </c>
+      <c r="S19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="11"/>
       <c r="E20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="11"/>
       <c r="I20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="8"/>
+      <c r="K20" s="14"/>
       <c r="M20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="N20" s="8" t="s">
+      <c r="N20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="O20" s="8"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O20" s="14"/>
+      <c r="Q20" t="s">
+        <v>49</v>
+      </c>
+      <c r="S20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="11"/>
       <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="11"/>
       <c r="I21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="6"/>
+      <c r="K21" s="8"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="11"/>
       <c r="E22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="G22" s="11"/>
       <c r="I22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K22" s="6"/>
+      <c r="K22" s="8"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="11"/>
       <c r="E23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="6"/>
+      <c r="G23" s="8"/>
       <c r="I23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="5"/>
+      <c r="K23" s="11"/>
       <c r="M23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O23" s="11"/>
+      <c r="Q23" t="s">
+        <v>66</v>
+      </c>
+      <c r="S23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="11"/>
       <c r="E24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="11"/>
       <c r="I24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="5"/>
+      <c r="K24" s="11"/>
       <c r="M24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="O24" s="11"/>
+      <c r="Q24" t="s">
+        <v>67</v>
+      </c>
+      <c r="S24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
         <v>2011</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="E25" s="7">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="E25" s="9">
         <v>2012</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
       <c r="I25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="5"/>
+      <c r="K25" s="11"/>
       <c r="M25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O25" s="11"/>
+      <c r="Q25" t="s">
+        <v>68</v>
+      </c>
+      <c r="S25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="5"/>
+      <c r="K26" s="11"/>
       <c r="M26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="O26" s="5"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O26" s="11"/>
+      <c r="Q26" t="s">
+        <v>69</v>
+      </c>
+      <c r="S26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K27" s="8"/>
-      <c r="M27" s="15" t="s">
+      <c r="K27" s="14"/>
+      <c r="M27" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N27" s="16" t="s">
+      <c r="N27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="O27" s="16"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O27" s="12"/>
+      <c r="Q27" t="s">
+        <v>70</v>
+      </c>
+      <c r="S27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="6" t="s">
+      <c r="J28" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K28" s="6"/>
-      <c r="M28" s="10" t="s">
+      <c r="K28" s="8"/>
+      <c r="M28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N28" s="11" t="s">
+      <c r="N28" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="O28" s="11"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O28" s="13"/>
+      <c r="Q28" t="s">
+        <v>59</v>
+      </c>
+      <c r="S28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="J29" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="K29" s="6"/>
-      <c r="M29" s="10" t="s">
+      <c r="K29" s="8"/>
+      <c r="M29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I30" s="7">
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="Q29" t="s">
+        <v>52</v>
+      </c>
+      <c r="S29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I30" s="9">
         <v>2013</v>
       </c>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="M30" s="10" t="s">
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="M30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="Q30" t="s">
+        <v>53</v>
+      </c>
+      <c r="S30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="M31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N31" s="6" t="s">
+      <c r="N31" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="O31" s="6"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M32" s="7">
+      <c r="O31" s="8"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M32" s="9">
         <v>2019</v>
       </c>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
@@ -1423,51 +1720,537 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063A7CB1-02AE-40E8-9AFC-D8E349A1BDD3}">
+  <dimension ref="B2:F45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>2019</v>
+      </c>
+      <c r="D2">
+        <v>2015</v>
+      </c>
+      <c r="F2">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
+        <v>97</v>
+      </c>
+      <c r="F38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
nacimientos 2013 y 2014
</commit_message>
<xml_diff>
--- a/xlsx/AnalisisVariablesProyecto.xlsx
+++ b/xlsx/AnalisisVariablesProyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\GIT\Proyecto-analisis-y-clustering\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7adc98a74669935/Documents/Clases/Mineria de datos/Proyecto-analisis-y-clustering/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AD27DE-3DE4-4D84-9F8D-0CD333D6058C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{61AD27DE-3DE4-4D84-9F8D-0CD333D6058C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFFA8600-1D5D-4916-8C25-58B6D5E98D90}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="13848" yWindow="1620" windowWidth="8736" windowHeight="9564" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="122">
   <si>
     <t>Depreg</t>
   </si>
@@ -344,13 +344,61 @@
   </si>
   <si>
     <t>PURBLOPP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naciop </t>
+  </si>
+  <si>
+    <t>escolap</t>
+  </si>
+  <si>
+    <t>ciupad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naciom </t>
+  </si>
+  <si>
+    <t>ciumad</t>
+  </si>
+  <si>
+    <t>Ocupación subgrupos CIUO-08 de la madre</t>
+  </si>
+  <si>
+    <t>Naciondalida de la madre</t>
+  </si>
+  <si>
+    <t>Ocupación subgrupos CIUO-08 del padre</t>
+  </si>
+  <si>
+    <t>escolaridad del padre</t>
+  </si>
+  <si>
+    <t>Naciondalida del padre</t>
+  </si>
+  <si>
+    <t>ocupacion del padre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ciumad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">anio de ocurrencia </t>
+  </si>
+  <si>
+    <t>via del parto</t>
+  </si>
+  <si>
+    <t>ocupacion de la madre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipo de inscripcion </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,8 +457,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +490,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -448,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -469,17 +536,26 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,15 +563,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,10 +849,10 @@
   <dimension ref="A4:S32"/>
   <sheetViews>
     <sheetView topLeftCell="N6" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+      <selection activeCell="N20" sqref="N20:O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.109375" style="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
@@ -795,31 +865,31 @@
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="12"/>
       <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="12"/>
       <c r="I4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="16"/>
+      <c r="K4" s="12"/>
       <c r="M4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="16"/>
+      <c r="O4" s="12"/>
       <c r="Q4" t="s">
         <v>54</v>
       </c>
@@ -831,31 +901,31 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="8"/>
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="G5" s="8"/>
       <c r="I5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="11"/>
+      <c r="K5" s="8"/>
       <c r="M5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="11"/>
+      <c r="O5" s="8"/>
       <c r="Q5" t="s">
         <v>55</v>
       </c>
@@ -867,31 +937,31 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="8"/>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="8"/>
       <c r="I6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="8"/>
       <c r="M6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="11"/>
+      <c r="O6" s="8"/>
       <c r="Q6" t="s">
         <v>56</v>
       </c>
@@ -903,31 +973,31 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="8"/>
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="8"/>
       <c r="I7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="11"/>
+      <c r="K7" s="8"/>
       <c r="M7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="11"/>
+      <c r="O7" s="8"/>
       <c r="Q7" t="s">
         <v>57</v>
       </c>
@@ -939,31 +1009,31 @@
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="8"/>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="G8" s="8"/>
       <c r="I8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="11"/>
+      <c r="K8" s="8"/>
       <c r="M8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="N8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="11"/>
+      <c r="O8" s="8"/>
       <c r="Q8" t="s">
         <v>58</v>
       </c>
@@ -975,31 +1045,31 @@
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="8"/>
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="8"/>
       <c r="I9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="11"/>
+      <c r="K9" s="8"/>
       <c r="M9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="N9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="11"/>
+      <c r="O9" s="8"/>
       <c r="Q9" t="s">
         <v>60</v>
       </c>
@@ -1011,31 +1081,31 @@
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="8"/>
       <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="11"/>
+      <c r="G10" s="8"/>
       <c r="I10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="11"/>
+      <c r="K10" s="8"/>
       <c r="M10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="N10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="11"/>
+      <c r="O10" s="8"/>
       <c r="Q10" t="s">
         <v>61</v>
       </c>
@@ -1047,31 +1117,31 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="8"/>
       <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="11"/>
+      <c r="G11" s="8"/>
       <c r="I11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="9"/>
+      <c r="K11" s="11"/>
       <c r="M11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N11" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="15"/>
+      <c r="O11" s="13"/>
       <c r="Q11" t="s">
         <v>43</v>
       </c>
@@ -1083,31 +1153,31 @@
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="8"/>
       <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="8"/>
       <c r="I12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="9"/>
+      <c r="K12" s="11"/>
       <c r="M12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="N12" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="O12" s="15"/>
+      <c r="O12" s="13"/>
       <c r="Q12" t="s">
         <v>45</v>
       </c>
@@ -1119,83 +1189,83 @@
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="8"/>
       <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="8"/>
       <c r="I13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="8"/>
+      <c r="K13" s="10"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="8"/>
       <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="8"/>
       <c r="I14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="8"/>
+      <c r="K14" s="10"/>
       <c r="M14" s="3"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="8"/>
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="8"/>
       <c r="I15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="11"/>
+      <c r="K15" s="8"/>
       <c r="M15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N15" s="11" t="s">
+      <c r="N15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O15" s="11"/>
+      <c r="O15" s="8"/>
       <c r="Q15" t="s">
         <v>62</v>
       </c>
@@ -1207,31 +1277,31 @@
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="8"/>
       <c r="E16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="G16" s="8"/>
       <c r="I16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="11"/>
+      <c r="K16" s="8"/>
       <c r="M16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="N16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O16" s="11"/>
+      <c r="O16" s="8"/>
       <c r="Q16" t="s">
         <v>63</v>
       </c>
@@ -1243,31 +1313,31 @@
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="8"/>
       <c r="E17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="8"/>
       <c r="I17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="11"/>
+      <c r="K17" s="8"/>
       <c r="M17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="N17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O17" s="11"/>
+      <c r="O17" s="8"/>
       <c r="Q17" t="s">
         <v>64</v>
       </c>
@@ -1279,31 +1349,31 @@
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="8"/>
       <c r="E18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="8"/>
       <c r="I18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="11"/>
+      <c r="K18" s="8"/>
       <c r="M18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N18" s="11" t="s">
+      <c r="N18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O18" s="11"/>
+      <c r="O18" s="8"/>
       <c r="Q18" t="s">
         <v>65</v>
       </c>
@@ -1315,31 +1385,31 @@
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="8"/>
       <c r="E19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="11"/>
+      <c r="G19" s="8"/>
       <c r="I19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="14"/>
+      <c r="K19" s="9"/>
       <c r="M19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N19" s="14" t="s">
+      <c r="N19" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="O19" s="14"/>
+      <c r="O19" s="9"/>
       <c r="Q19" t="s">
         <v>47</v>
       </c>
@@ -1351,31 +1421,31 @@
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="8"/>
       <c r="E20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="11"/>
+      <c r="G20" s="8"/>
       <c r="I20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="14"/>
+      <c r="K20" s="9"/>
       <c r="M20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="N20" s="14" t="s">
+      <c r="N20" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="O20" s="14"/>
+      <c r="O20" s="9"/>
       <c r="Q20" t="s">
         <v>49</v>
       </c>
@@ -1387,83 +1457,83 @@
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="8"/>
       <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="11"/>
+      <c r="G21" s="8"/>
       <c r="I21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="8"/>
+      <c r="K21" s="10"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="8"/>
       <c r="E22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="11"/>
+      <c r="G22" s="8"/>
       <c r="I22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K22" s="8"/>
+      <c r="K22" s="10"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="8"/>
       <c r="E23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="8"/>
+      <c r="G23" s="10"/>
       <c r="I23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J23" s="11" t="s">
+      <c r="J23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="11"/>
+      <c r="K23" s="8"/>
       <c r="M23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N23" s="11" t="s">
+      <c r="N23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="O23" s="11"/>
+      <c r="O23" s="8"/>
       <c r="Q23" t="s">
         <v>66</v>
       </c>
@@ -1475,31 +1545,31 @@
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="8"/>
       <c r="E24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="11"/>
+      <c r="G24" s="8"/>
       <c r="I24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="J24" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="11"/>
+      <c r="K24" s="8"/>
       <c r="M24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N24" s="11" t="s">
+      <c r="N24" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="11"/>
+      <c r="O24" s="8"/>
       <c r="Q24" t="s">
         <v>67</v>
       </c>
@@ -1508,30 +1578,30 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
+      <c r="A25" s="11">
         <v>2011</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="E25" s="9">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="E25" s="11">
         <v>2012</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
       <c r="I25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="11"/>
+      <c r="K25" s="8"/>
       <c r="M25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N25" s="11" t="s">
+      <c r="N25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="11"/>
+      <c r="O25" s="8"/>
       <c r="Q25" t="s">
         <v>68</v>
       </c>
@@ -1543,17 +1613,17 @@
       <c r="I26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="J26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="11"/>
+      <c r="K26" s="8"/>
       <c r="M26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N26" s="11" t="s">
+      <c r="N26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="O26" s="11"/>
+      <c r="O26" s="8"/>
       <c r="Q26" t="s">
         <v>69</v>
       </c>
@@ -1565,17 +1635,17 @@
       <c r="I27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="K27" s="14"/>
+      <c r="K27" s="9"/>
       <c r="M27" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N27" s="12" t="s">
+      <c r="N27" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="O27" s="12"/>
+      <c r="O27" s="15"/>
       <c r="Q27" t="s">
         <v>70</v>
       </c>
@@ -1587,17 +1657,17 @@
       <c r="I28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K28" s="8"/>
+      <c r="K28" s="10"/>
       <c r="M28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="N28" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="O28" s="13"/>
+      <c r="O28" s="16"/>
       <c r="Q28" t="s">
         <v>59</v>
       </c>
@@ -1609,15 +1679,15 @@
       <c r="I29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J29" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K29" s="8"/>
+      <c r="K29" s="10"/>
       <c r="M29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
       <c r="Q29" t="s">
         <v>52</v>
       </c>
@@ -1626,16 +1696,16 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I30" s="9">
+      <c r="I30" s="11">
         <v>2013</v>
       </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
       <c r="M30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
       <c r="Q30" t="s">
         <v>53</v>
       </c>
@@ -1647,63 +1717,61 @@
       <c r="M31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N31" s="8" t="s">
+      <c r="N31" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="O31" s="8"/>
+      <c r="O31" s="10"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="M32" s="9">
+      <c r="M32" s="11">
         <v>2019</v>
       </c>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
@@ -1720,47 +1788,49 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1769,15 +1839,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063A7CB1-02AE-40E8-9AFC-D8E349A1BDD3}">
-  <dimension ref="B2:F45"/>
+  <dimension ref="B2:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="25.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="13" max="13" width="28.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>2019</v>
       </c>
@@ -1787,8 +1862,14 @@
       <c r="F2">
         <v>2016</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>2013</v>
+      </c>
+      <c r="K2">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -1798,8 +1879,14 @@
       <c r="F4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -1809,8 +1896,14 @@
       <c r="F5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H5" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>56</v>
       </c>
@@ -1820,8 +1913,14 @@
       <c r="F6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>57</v>
       </c>
@@ -1831,8 +1930,14 @@
       <c r="F7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H7" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>71</v>
       </c>
@@ -1842,8 +1947,17 @@
       <c r="F8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>66</v>
       </c>
@@ -1853,8 +1967,14 @@
       <c r="F9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>67</v>
       </c>
@@ -1864,8 +1984,14 @@
       <c r="F10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H10" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>72</v>
       </c>
@@ -1875,8 +2001,14 @@
       <c r="F11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H11" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>73</v>
       </c>
@@ -1886,8 +2018,14 @@
       <c r="F12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H12" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>74</v>
       </c>
@@ -1897,8 +2035,14 @@
       <c r="F13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H13" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>69</v>
       </c>
@@ -1908,8 +2052,14 @@
       <c r="F14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H14" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>59</v>
       </c>
@@ -1919,8 +2069,17 @@
       <c r="F15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" t="s">
+        <v>118</v>
+      </c>
+      <c r="K15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>75</v>
       </c>
@@ -1930,8 +2089,14 @@
       <c r="F16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H16" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>76</v>
       </c>
@@ -1941,8 +2106,14 @@
       <c r="F17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H17" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>77</v>
       </c>
@@ -1952,8 +2123,17 @@
       <c r="F18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" t="s">
+        <v>119</v>
+      </c>
+      <c r="K18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>78</v>
       </c>
@@ -1963,8 +2143,14 @@
       <c r="F19" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H19" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>79</v>
       </c>
@@ -1974,8 +2160,14 @@
       <c r="F20" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H20" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>80</v>
       </c>
@@ -1985,8 +2177,14 @@
       <c r="F21" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H21" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>81</v>
       </c>
@@ -1996,8 +2194,14 @@
       <c r="F22" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H22" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>82</v>
       </c>
@@ -2007,8 +2211,14 @@
       <c r="F23" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H23" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>83</v>
       </c>
@@ -2018,8 +2228,14 @@
       <c r="F24" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H24" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>84</v>
       </c>
@@ -2029,8 +2245,14 @@
       <c r="F25" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H25" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>85</v>
       </c>
@@ -2040,8 +2262,14 @@
       <c r="F26" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H26" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>86</v>
       </c>
@@ -2051,8 +2279,14 @@
       <c r="F27" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H27" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>87</v>
       </c>
@@ -2062,8 +2296,14 @@
       <c r="F28" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H28" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>88</v>
       </c>
@@ -2073,8 +2313,17 @@
       <c r="F29" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" t="s">
+        <v>116</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>89</v>
       </c>
@@ -2084,8 +2333,14 @@
       <c r="F30" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H30" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>90</v>
       </c>
@@ -2095,8 +2350,14 @@
       <c r="F31" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H31" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>91</v>
       </c>
@@ -2106,8 +2367,14 @@
       <c r="F32" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H32" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>92</v>
       </c>
@@ -2117,8 +2384,14 @@
       <c r="F33" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H33" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>93</v>
       </c>
@@ -2128,8 +2401,14 @@
       <c r="F34" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H34" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>94</v>
       </c>
@@ -2139,8 +2418,14 @@
       <c r="F35" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H35" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>95</v>
       </c>
@@ -2150,8 +2435,14 @@
       <c r="F36" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H36" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>96</v>
       </c>
@@ -2161,8 +2452,14 @@
       <c r="F37" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H37" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>97</v>
       </c>
@@ -2172,8 +2469,14 @@
       <c r="F38" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H38" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>98</v>
       </c>
@@ -2183,8 +2486,14 @@
       <c r="F39" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H39" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>99</v>
       </c>
@@ -2194,8 +2503,17 @@
       <c r="F40" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>99</v>
+      </c>
+      <c r="I40" t="s">
+        <v>120</v>
+      </c>
+      <c r="K40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>100</v>
       </c>
@@ -2205,8 +2523,14 @@
       <c r="F41" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H41" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>101</v>
       </c>
@@ -2216,8 +2540,14 @@
       <c r="F42" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H42" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>102</v>
       </c>
@@ -2227,8 +2557,14 @@
       <c r="F43" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H43" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>103</v>
       </c>
@@ -2238,8 +2574,14 @@
       <c r="F44" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H44" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>104</v>
       </c>
@@ -2249,8 +2591,69 @@
       <c r="F45" t="s">
         <v>104</v>
       </c>
+      <c r="H45" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="K45" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H46" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I46" t="s">
+        <v>115</v>
+      </c>
+      <c r="K46" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="M46" s="9"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H47" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H48" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J48" s="9"/>
+    </row>
+    <row r="49" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H49" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="I49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H50" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J50" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="L46:M46"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>